<commit_message>
# amended errors in file
</commit_message>
<xml_diff>
--- a/SiPy Commands.xlsx
+++ b/SiPy Commands.xlsx
@@ -5,20 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maurice\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenttpedu-my.sharepoint.com/personal/maurice_tp_edu_sg/Documents/Projects/sipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2766591-AF51-4D7A-BF1E-A19F3EA82502}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="147">
   <si>
     <t xml:space="preserve">List or Dataframe </t>
   </si>
@@ -110,48 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">skipped </t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    Pearson    list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    Pearson    dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    spearman     list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    spearman     dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    kendall    list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    kendall    dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    bicor    list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    bicor    dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    percbend    list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    percbend    dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    shepherd    list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    shepherd    dataframewide z x y</t>
-  </si>
-  <si>
-    <t>let x be list 2,3,4,5,6,7,8,9 let y be list 3,4,5,6,7,8,9,10   Correlate    skipped     list x y</t>
-  </si>
-  <si>
-    <t>let x be list 1,2,3,4,5 let y be list 2,3,4,5,6   let z be dataframe x:x y:yCorrelate    skipped     dataframewide z x y</t>
   </si>
   <si>
     <t>let x be list 1,2,3,4,5
@@ -193,19 +149,9 @@
     <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">let x be list 1,2,3,4,5
-let y be list 2,3,4,5,6
-let z be dataframe x:x y:y
-correlate bicor dataframe wide z x y
-</t>
-  </si>
-  <si>
     <t>let x be list 2,3,4,5,6,7,8,9
 let y be list 3,4,5,6,7,8,9,10
 correlate  shepherd list x y</t>
-  </si>
-  <si>
-    <t>Distance</t>
   </si>
   <si>
     <t>let x be list 2,3,4,5,6,7,8,9
@@ -647,6 +593,86 @@
 let y be list 2,3,4,5,6
 let z be dataframe x:x y:y
 correlate CV2 dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+correlate bicor dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize r dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize r list x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+correlate bicor list x y</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize auc list x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize cles list x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize cles dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize auc dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize eta-square dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize eta-square list x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize odds-ratio list x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize odds-ratio dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+compute_effsize pointbiserialr dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+compute_effsize pointbiserialr list x y</t>
   </si>
 </sst>
 </file>
@@ -728,7 +754,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1059,11 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,36 +1144,36 @@
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
@@ -1117,719 +1182,719 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E24" s="4">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="E30" s="4">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="E31" s="4">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="E34" s="4">
+        <v>3</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="4">
-        <v>1</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="E35" s="4">
+        <v>3</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="4">
-        <v>1</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E36" s="4">
+        <v>3</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="4">
-        <v>1</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="4">
-        <v>2</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="4">
-        <v>2</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="4">
-        <v>2</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="4">
-        <v>2</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="4">
-        <v>3</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="4">
-        <v>3</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="4">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="4">
-        <v>3</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="4">
-        <v>3</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="4">
-        <v>3</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="E37" s="4">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="4">
-        <v>3</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="4">
-        <v>3</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="4">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" s="4">
-        <v>3</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="4">
-        <v>3</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E38" s="4">
         <v>3</v>
       </c>
@@ -1837,7 +1902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
@@ -1848,7 +1913,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E39" s="4">
         <v>4</v>
@@ -1862,13 +1927,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E40" s="4">
         <v>4</v>
@@ -1877,7 +1942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1888,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E41" s="4">
         <v>4</v>
@@ -1902,13 +1967,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E42" s="4">
         <v>4</v>
@@ -1917,7 +1982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
@@ -1925,10 +1990,10 @@
         <v>6</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E43" s="4">
         <v>4</v>
@@ -1937,18 +2002,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E44" s="4">
         <v>4</v>
@@ -1957,7 +2022,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
@@ -1965,10 +2030,10 @@
         <v>10</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E45" s="4">
         <v>4</v>
@@ -1977,18 +2042,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E46" s="4">
         <v>4</v>
@@ -1997,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -2005,10 +2070,10 @@
         <v>7</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E47" s="4">
         <v>4</v>
@@ -2017,18 +2082,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E48" s="4">
         <v>4</v>
@@ -2037,7 +2102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
@@ -2045,10 +2110,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E49" s="4">
         <v>4</v>
@@ -2062,13 +2127,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E50" s="4">
         <v>4</v>
@@ -2077,7 +2142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>4</v>
       </c>
@@ -2088,7 +2153,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E51" s="4">
         <v>4</v>
@@ -2102,13 +2167,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E52" s="4">
         <v>4</v>
@@ -2117,7 +2182,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>4</v>
       </c>
@@ -2125,31 +2190,31 @@
         <v>8</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D53" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="4">
+        <v>4</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="4">
-        <v>4</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E54" s="4">
         <v>4</v>
       </c>
@@ -2157,18 +2222,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E55" s="4">
         <v>4</v>
@@ -2177,18 +2242,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E56" s="4">
         <v>4</v>
@@ -2202,13 +2267,13 @@
         <v>15</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="E57" s="4">
         <v>4</v>
@@ -2222,13 +2287,13 @@
         <v>15</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E58" s="4">
         <v>4</v>
@@ -2242,13 +2307,13 @@
         <v>15</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="E59" s="4">
         <v>4</v>
@@ -2262,13 +2327,13 @@
         <v>15</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E60" s="4">
         <v>4</v>
@@ -2282,13 +2347,13 @@
         <v>15</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E61" s="4">
         <v>4</v>
@@ -2302,13 +2367,13 @@
         <v>15</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E62" s="4">
         <v>4</v>
@@ -2322,13 +2387,13 @@
         <v>15</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="E63" s="4">
         <v>4</v>
@@ -2342,13 +2407,13 @@
         <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E64" s="4">
         <v>4</v>
@@ -2362,13 +2427,13 @@
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E65" s="4">
         <v>4</v>
@@ -2382,13 +2447,13 @@
         <v>15</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E66" s="4">
         <v>4</v>
@@ -2399,16 +2464,16 @@
     </row>
     <row r="67" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>112</v>
+      <c r="D67" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="E67" s="4">
         <v>4</v>
@@ -2419,16 +2484,16 @@
     </row>
     <row r="68" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="E68" s="4">
         <v>4</v>
@@ -2439,16 +2504,16 @@
     </row>
     <row r="69" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="E69" s="4">
         <v>4</v>
@@ -2459,16 +2524,16 @@
     </row>
     <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="E70" s="4">
         <v>4</v>
@@ -2477,318 +2542,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="4">
+        <v>4</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E72" s="4">
+        <v>4</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E71" s="4">
-        <v>4</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E72" s="4">
-        <v>4</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C73" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E73" s="4">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E74" s="4">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E75" s="4">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E76" s="4">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E77" s="4">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E78" s="4">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E79" s="4">
-        <v>4</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>44</v>
+      <c r="C80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F79" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="4"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F79">
-    <sortCondition ref="E2:E79"/>
-    <sortCondition descending="1" ref="F2:F79"/>
-    <sortCondition ref="A2:A79"/>
-    <sortCondition ref="B2:B79"/>
-    <sortCondition ref="C2:C79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F81">
+    <sortCondition ref="E2:E81"/>
+    <sortCondition descending="1" ref="F2:F81"/>
+    <sortCondition ref="A2:A81"/>
+    <sortCondition ref="B2:B81"/>
+    <sortCondition ref="C2:C81"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F79">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+  <conditionalFormatting sqref="F2:F38 F56:F81 F40:F54">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F55">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F55)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F39)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A6FFE3-A99E-44D4-B73A-21D22C5725B0}">
-  <dimension ref="A1:A14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:A16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="101.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FABD2F-70F2-480B-8B56-13CE8C832736}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
+ added 1-way repeated measures ANOVA from dataframe (wide)
</commit_message>
<xml_diff>
--- a/SiPy Commands.xlsx
+++ b/SiPy Commands.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenttpedu-my.sharepoint.com/personal/maurice_tp_edu_sg/Documents/Projects/sipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2766591-AF51-4D7A-BF1E-A19F3EA82502}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE62C99B-E69E-4284-A834-2561E4568219}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
+    <workbookView xWindow="5610" yWindow="220" windowWidth="13030" windowHeight="9680" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="149">
   <si>
     <t xml:space="preserve">List or Dataframe </t>
   </si>
@@ -673,6 +673,15 @@
     <t>let x be list 2,3,4,5,6,7,8,9
 let y be list 3,4,5,6,7,8,9,10
 compute_effsize pointbiserialr list x y</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let z be dataframe X1:X1 X2:X2
+anova rm dataframe wide z</t>
   </si>
 </sst>
 </file>
@@ -754,7 +763,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1125,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1682,21 +1711,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>148</v>
       </c>
       <c r="E28" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>3</v>
@@ -1707,13 +1736,13 @@
         <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E29" s="4">
         <v>3</v>
@@ -1727,13 +1756,13 @@
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E30" s="4">
         <v>3</v>
@@ -1747,33 +1776,33 @@
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E31" s="4">
-        <v>3</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E32" s="4">
         <v>3</v>
@@ -1787,13 +1816,13 @@
         <v>80</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E33" s="4">
         <v>3</v>
@@ -1807,13 +1836,13 @@
         <v>80</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E34" s="4">
         <v>3</v>
@@ -1827,33 +1856,33 @@
         <v>80</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="4">
+        <v>3</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E35" s="4">
-        <v>3</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E36" s="4">
         <v>3</v>
@@ -1867,13 +1896,13 @@
         <v>42</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E37" s="4">
         <v>3</v>
@@ -1887,42 +1916,42 @@
         <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="4">
-        <v>3</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E39" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -1930,10 +1959,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E40" s="4">
         <v>4</v>
@@ -1947,13 +1976,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E41" s="4">
         <v>4</v>
@@ -1962,7 +1991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
@@ -1970,10 +1999,10 @@
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E42" s="4">
         <v>4</v>
@@ -1987,13 +2016,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="E43" s="4">
         <v>4</v>
@@ -2002,7 +2031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
@@ -2010,31 +2039,31 @@
         <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="4">
-        <v>4</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="E45" s="4">
         <v>4</v>
       </c>
@@ -2042,7 +2071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
@@ -2050,31 +2079,31 @@
         <v>10</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E46" s="4">
+        <v>4</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E46" s="4">
-        <v>4</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E47" s="4">
         <v>4</v>
       </c>
@@ -2082,7 +2111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>4</v>
       </c>
@@ -2090,31 +2119,31 @@
         <v>7</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="4">
+        <v>4</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="4">
-        <v>4</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="E49" s="4">
         <v>4</v>
       </c>
@@ -2122,7 +2151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>4</v>
       </c>
@@ -2130,10 +2159,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E50" s="4">
         <v>4</v>
@@ -2147,13 +2176,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="E51" s="4">
         <v>4</v>
@@ -2162,7 +2191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>4</v>
       </c>
@@ -2173,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E52" s="4">
         <v>4</v>
@@ -2187,13 +2216,13 @@
         <v>4</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E53" s="4">
         <v>4</v>
@@ -2202,7 +2231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>4</v>
       </c>
@@ -2210,10 +2239,10 @@
         <v>8</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E54" s="4">
         <v>4</v>
@@ -2224,16 +2253,16 @@
     </row>
     <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>135</v>
+      <c r="D55" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="E55" s="4">
         <v>4</v>
@@ -2242,7 +2271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>15</v>
       </c>
@@ -2250,10 +2279,10 @@
         <v>19</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E56" s="4">
         <v>4</v>
@@ -2267,13 +2296,13 @@
         <v>15</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E57" s="4">
         <v>4</v>
@@ -2282,7 +2311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>15</v>
       </c>
@@ -2290,10 +2319,10 @@
         <v>136</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="E58" s="4">
         <v>4</v>
@@ -2302,18 +2331,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="E59" s="4">
         <v>4</v>
@@ -2322,7 +2351,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>15</v>
       </c>
@@ -2330,10 +2359,10 @@
         <v>18</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E60" s="4">
         <v>4</v>
@@ -2342,18 +2371,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>124</v>
+        <v>1</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E61" s="4">
         <v>4</v>
@@ -2362,7 +2391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>15</v>
       </c>
@@ -2370,10 +2399,10 @@
         <v>16</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="E62" s="4">
         <v>4</v>
@@ -2382,18 +2411,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>126</v>
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E63" s="4">
         <v>4</v>
@@ -2402,7 +2431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
@@ -2410,10 +2439,10 @@
         <v>20</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="E64" s="4">
         <v>4</v>
@@ -2422,18 +2451,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>128</v>
+        <v>1</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E65" s="4">
         <v>4</v>
@@ -2442,7 +2471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>15</v>
       </c>
@@ -2450,10 +2479,10 @@
         <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="E66" s="4">
         <v>4</v>
@@ -2462,18 +2491,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>125</v>
+        <v>1</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E67" s="4">
         <v>4</v>
@@ -2482,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>15</v>
       </c>
@@ -2490,31 +2519,31 @@
         <v>17</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E68" s="4">
+        <v>4</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E68" s="4">
-        <v>4</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="E69" s="4">
         <v>4</v>
       </c>
@@ -2522,7 +2551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>80</v>
       </c>
@@ -2530,10 +2559,10 @@
         <v>83</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E70" s="4">
         <v>4</v>
@@ -2542,18 +2571,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E71" s="4">
         <v>4</v>
@@ -2562,7 +2591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>80</v>
       </c>
@@ -2570,36 +2599,39 @@
         <v>85</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E72" s="4">
+        <v>4</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="4">
-        <v>4</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>145</v>
+      <c r="E73" s="4">
+        <v>4</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>4</v>
       </c>
@@ -2607,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>14</v>
@@ -2618,16 +2650,16 @@
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>14</v>
@@ -2638,13 +2670,13 @@
         <v>15</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>14</v>
@@ -2655,30 +2687,30 @@
         <v>15</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>130</v>
+        <v>1</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F78" s="4" t="s">
         <v>30</v>
@@ -2689,13 +2721,13 @@
         <v>15</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>30</v>
@@ -2706,19 +2738,19 @@
         <v>15</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>15</v>
       </c>
@@ -2726,46 +2758,71 @@
         <v>21</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="82" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F81">
-    <sortCondition ref="E2:E81"/>
-    <sortCondition descending="1" ref="F2:F81"/>
-    <sortCondition ref="A2:A81"/>
-    <sortCondition ref="B2:B81"/>
-    <sortCondition ref="C2:C81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F82">
+    <sortCondition ref="E2:E82"/>
+    <sortCondition descending="1" ref="F2:F82"/>
+    <sortCondition ref="A2:A82"/>
+    <sortCondition ref="B2:B82"/>
+    <sortCondition ref="C2:C82"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F38 F56:F81 F40:F54">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+  <conditionalFormatting sqref="F2:F27 F57:F82 F41:F55 F29:F39">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F55">
+  <conditionalFormatting sqref="F56">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F40">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("no",F40)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F55)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
+  <conditionalFormatting sqref="F28">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("no",F28)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F39)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+ added kwargs to commands (preparation for 0.5.0)
</commit_message>
<xml_diff>
--- a/SiPy Commands.xlsx
+++ b/SiPy Commands.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenttpedu-my.sharepoint.com/personal/maurice_tp_edu_sg/Documents/Projects/sipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE62C99B-E69E-4284-A834-2561E4568219}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{681DA11C-C568-4AF1-909E-9D07E2282F1E}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="220" windowWidth="13030" windowHeight="9680" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="151">
   <si>
     <t xml:space="preserve">List or Dataframe </t>
   </si>
@@ -682,6 +682,16 @@
 let X2 be list 2,3,4,5,6,7
 let z be dataframe X1:X1 X2:X2
 anova rm dataframe wide z</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+ttest 1s list data=x mu=4</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest 1s dataframe wide data=z.x mu=5</t>
   </si>
 </sst>
 </file>
@@ -763,7 +773,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1154,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1491,21 +1541,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>3</v>
@@ -1516,13 +1566,13 @@
         <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -1536,33 +1586,33 @@
         <v>80</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1576,13 +1626,13 @@
         <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1596,36 +1646,36 @@
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="E23" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>3</v>
@@ -1636,13 +1686,13 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24" s="4">
         <v>2</v>
@@ -1656,13 +1706,13 @@
         <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E25" s="4">
         <v>2</v>
@@ -1676,36 +1726,36 @@
         <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="4">
-        <v>2</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="E27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>3</v>
@@ -1716,36 +1766,36 @@
         <v>110</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="4">
-        <v>4</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E29" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>3</v>
@@ -1756,13 +1806,13 @@
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E30" s="4">
         <v>3</v>
@@ -1776,13 +1826,13 @@
         <v>56</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E31" s="4">
         <v>3</v>
@@ -1796,33 +1846,33 @@
         <v>56</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="E32" s="4">
-        <v>3</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="E33" s="4">
         <v>3</v>
@@ -1836,13 +1886,13 @@
         <v>80</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E34" s="4">
         <v>3</v>
@@ -1856,16 +1906,16 @@
         <v>80</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="E35" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>3</v>
@@ -1876,53 +1926,53 @@
         <v>80</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="C38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E36" s="4">
-        <v>3</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" s="4">
-        <v>3</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E38" s="4">
         <v>3</v>
@@ -1936,133 +1986,133 @@
         <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="4">
+        <v>3</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="4">
+        <v>3</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="4">
-        <v>3</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="E41" s="4">
+        <v>3</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3" t="s">
+      <c r="C42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E40" s="4">
-        <v>4</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="E42" s="4">
+        <v>4</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E41" s="4">
-        <v>4</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="E43" s="4">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="C44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="4">
-        <v>4</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="C45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="E43" s="4">
-        <v>4</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E44" s="4">
-        <v>4</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E45" s="4">
         <v>4</v>
@@ -2076,13 +2126,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="E46" s="4">
         <v>4</v>
@@ -2096,13 +2146,13 @@
         <v>4</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E47" s="4">
         <v>4</v>
@@ -2116,13 +2166,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E48" s="4">
         <v>4</v>
@@ -2136,13 +2186,13 @@
         <v>4</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="E49" s="4">
         <v>4</v>
@@ -2156,13 +2206,13 @@
         <v>4</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E50" s="4">
         <v>4</v>
@@ -2176,134 +2226,134 @@
         <v>4</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="4">
+        <v>4</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="3" t="s">
+      <c r="C52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E52" s="4">
+        <v>4</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="4">
-        <v>4</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="E53" s="4">
+        <v>4</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E52" s="4">
-        <v>4</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="2" t="s">
+      <c r="E54" s="4">
+        <v>4</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="3" t="s">
+      <c r="C55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="4">
-        <v>4</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="2" t="s">
+      <c r="E55" s="4">
+        <v>4</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D54" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E54" s="4">
-        <v>4</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="2" t="s">
+      <c r="E56" s="4">
+        <v>4</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="C57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E55" s="4">
-        <v>4</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="4">
-        <v>4</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="E57" s="4">
         <v>4</v>
       </c>
@@ -2311,18 +2361,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E58" s="4">
         <v>4</v>
@@ -2331,18 +2381,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E59" s="4">
         <v>4</v>
@@ -2356,13 +2406,13 @@
         <v>15</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="E60" s="4">
         <v>4</v>
@@ -2376,13 +2426,13 @@
         <v>15</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E61" s="4">
         <v>4</v>
@@ -2396,13 +2446,13 @@
         <v>15</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>124</v>
+        <v>23</v>
       </c>
       <c r="E62" s="4">
         <v>4</v>
@@ -2416,13 +2466,13 @@
         <v>15</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E63" s="4">
         <v>4</v>
@@ -2436,13 +2486,13 @@
         <v>15</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E64" s="4">
         <v>4</v>
@@ -2456,13 +2506,13 @@
         <v>15</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E65" s="4">
         <v>4</v>
@@ -2476,13 +2526,13 @@
         <v>15</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E66" s="4">
         <v>4</v>
@@ -2496,13 +2546,13 @@
         <v>15</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E67" s="4">
         <v>4</v>
@@ -2516,13 +2566,13 @@
         <v>15</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E68" s="4">
         <v>4</v>
@@ -2536,13 +2586,13 @@
         <v>15</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E69" s="4">
         <v>4</v>
@@ -2553,16 +2603,16 @@
     </row>
     <row r="70" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>96</v>
+      <c r="D70" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="E70" s="4">
         <v>4</v>
@@ -2573,16 +2623,16 @@
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="E71" s="4">
         <v>4</v>
@@ -2596,13 +2646,13 @@
         <v>80</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E72" s="4">
         <v>4</v>
@@ -2616,67 +2666,73 @@
         <v>80</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" s="4">
+        <v>4</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E73" s="4">
-        <v>4</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C74" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>145</v>
+        <v>98</v>
+      </c>
+      <c r="E74" s="4">
+        <v>4</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E75" s="4">
+        <v>4</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C76" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>14</v>
@@ -2684,16 +2740,16 @@
     </row>
     <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>14</v>
@@ -2704,47 +2760,47 @@
         <v>15</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>130</v>
+        <v>1</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>131</v>
+        <v>1</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>30</v>
@@ -2755,74 +2811,116 @@
         <v>15</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="F82" s="4" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="83" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F82">
-    <sortCondition ref="E2:E82"/>
-    <sortCondition descending="1" ref="F2:F82"/>
-    <sortCondition ref="A2:A82"/>
-    <sortCondition ref="B2:B82"/>
-    <sortCondition ref="C2:C82"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
+    <sortCondition ref="E2:E84"/>
+    <sortCondition descending="1" ref="F2:F84"/>
+    <sortCondition ref="A2:A84"/>
+    <sortCondition ref="B2:B84"/>
+    <sortCondition ref="C2:C84"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F27 F57:F82 F41:F55 F29:F39">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+  <conditionalFormatting sqref="F2:F28 F59:F84 F43:F57 F30:F34 F36:F41">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F56">
+  <conditionalFormatting sqref="F58">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F29">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("no",F29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
+  <conditionalFormatting sqref="F35">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("no",F35)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F28)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+ completed keyword arguments for ttest
</commit_message>
<xml_diff>
--- a/SiPy Commands.xlsx
+++ b/SiPy Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenttpedu-my.sharepoint.com/personal/maurice_tp_edu_sg/Documents/Projects/sipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{681DA11C-C568-4AF1-909E-9D07E2282F1E}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E681D129-C1CD-42D6-91CD-BB696A2B5365}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="166">
   <si>
     <t xml:space="preserve">List or Dataframe </t>
   </si>
@@ -692,6 +692,86 @@
 let y be list 2,3,4,5,6
 let z be dataframe x:x y:y
 ttest 1s dataframe wide data=z.x mu=5</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest 2se list data=x;y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest 2se dataframe wide data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest 2su list data=x;y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest 2su dataframe wide data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest mwu dataframe wide data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest mwu list data=x;y</t>
+  </si>
+  <si>
+    <t>tost</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest tost dataframe wide z x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest tost list x y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest paired list data=x;y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest paired dataframe data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest wilcoxon dataframe wide data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest wilcoxon list data=x;y</t>
+  </si>
+  <si>
+    <t>let x be list 1,2,3,4,5
+let y be list 2,3,4,5,6
+let z be dataframe x:x y:y
+ttest tost dataframe wide data=z.x;z.y</t>
+  </si>
+  <si>
+    <t>let x be list 2,3,4,5,6,7,8,9
+let y be list 3,4,5,6,7,8,9,10
+ttest tost list data=x;y</t>
   </si>
 </sst>
 </file>
@@ -773,7 +853,207 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1204,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2874,6 +3154,286 @@
         <v>30</v>
       </c>
     </row>
+    <row r="85" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E85" s="4">
+        <v>5</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E86" s="4">
+        <v>5</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E87" s="4">
+        <v>5</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A88" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E88" s="4">
+        <v>3</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E89" s="4">
+        <v>5</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E90" s="4">
+        <v>4</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" s="4">
+        <v>4</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E92" s="4">
+        <v>4</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E93" s="4">
+        <v>5</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E94" s="4">
+        <v>5</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E95" s="4">
+        <v>5</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E96" s="4">
+        <v>5</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E97" s="4">
+        <v>5</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E98" s="4">
+        <v>5</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
     <sortCondition ref="E2:E84"/>
@@ -2884,43 +3444,131 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2:F28 F59:F84 F43:F57 F30:F34 F36:F41">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F35)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F85">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F85)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F85)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F86">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F86)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F87">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F87)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F87)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F88">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F88)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F88)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F89">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F89)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F89)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F90">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F90)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F91:F92">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F91)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F93">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F93)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F93)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F94">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F95:F96">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F95)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F95)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97:F98">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F97)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+ completed keyword arguments for variance
</commit_message>
<xml_diff>
--- a/SiPy Commands.xlsx
+++ b/SiPy Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenttpedu-my.sharepoint.com/personal/maurice_tp_edu_sg/Documents/Projects/sipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E681D129-C1CD-42D6-91CD-BB696A2B5365}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{A4C9D013-DFA4-4CD8-A8DE-8CE64B95ED2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{972E6860-799C-43FC-9B46-D21CF3B04ADA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DC5DFBC8-E4EE-4037-8A51-252739BEA1CA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="172">
   <si>
     <t xml:space="preserve">List or Dataframe </t>
   </si>
@@ -772,6 +772,45 @@
     <t>let x be list 2,3,4,5,6,7,8,9
 let y be list 3,4,5,6,7,8,9,10
 ttest tost list data=x;y</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+variance bartlett list data=X1;X2;X3</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+let z be dataframe X1:X1 X2:X2 X3:X3
+variance bartlett frame wide data=z</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+variance fligner list data=X1;X2;X3</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+let z be dataframe X1:X1 X2:X2 X3:X3
+variance fligner frame wide data=z</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+variance levene list data=X1;X2;X3</t>
+  </si>
+  <si>
+    <t>let X1 be list 1,2,3,4,5,6
+let X2 be list 2,3,4,5,6,7
+let X3 be list 3,4,5,6,7,8
+let z be dataframe X1:X1 X2:X2 X3:X3
+variance levene frame wide data=z</t>
   </si>
 </sst>
 </file>
@@ -853,7 +892,127 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1484,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3434,7 +3593,128 @@
         <v>3</v>
       </c>
     </row>
+    <row r="99" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E99" s="4">
+        <v>5</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E100" s="4">
+        <v>5</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E101" s="4">
+        <v>5</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E102" s="4">
+        <v>5</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E103" s="4">
+        <v>5</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E104" s="4">
+        <v>5</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F104" xr:uid="{0F1B49D1-1790-4F90-A473-B1A1E4E7942C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F84">
     <sortCondition ref="E2:E84"/>
     <sortCondition descending="1" ref="F2:F84"/>
@@ -3444,131 +3724,179 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F2:F28 F59:F84 F43:F57 F30:F34 F36:F41">
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="43" priority="45" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F58)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42">
-    <cfRule type="containsText" dxfId="27" priority="29" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="38" priority="42" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F85">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="33" priority="33" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F85)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="32" priority="34" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F86">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F87">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F87)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F88">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F88)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F89">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F89)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F90">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F90)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F90)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F91:F92">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F93">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F94">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F94)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F95:F96">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",F95)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="Yes ">
       <formula>NOT(ISERROR(SEARCH("Yes ",F95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F97:F98">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F97)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F97)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F99">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F99)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F99)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F100">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F100)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F101">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F101)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F102">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F102)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F103">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="no">
+      <formula>NOT(ISERROR(SEARCH("no",F103)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Yes ">
+      <formula>NOT(ISERROR(SEARCH("Yes ",F103)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F104">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="no">
-      <formula>NOT(ISERROR(SEARCH("no",F97)))</formula>
+      <formula>NOT(ISERROR(SEARCH("no",F104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes ">
-      <formula>NOT(ISERROR(SEARCH("Yes ",F97)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes ",F104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>